<commit_message>
working on a tough two pointer problem
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E102C6-AD68-4851-868B-5344C4B190FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BE0D8-71EE-49A5-BAC4-6E316F82A73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>Permutation in String</t>
+  </si>
+  <si>
+    <t>04/06/2025</t>
+  </si>
+  <si>
+    <t>Tough One!!!</t>
+  </si>
+  <si>
+    <t>05/06/2025</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
   </si>
 </sst>
 </file>
@@ -301,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -321,13 +333,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,27 +669,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="83.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="83.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -713,7 +718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -739,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -765,7 +770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -791,7 +796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -817,7 +822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -846,7 +851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -872,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -901,7 +906,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -930,94 +935,94 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
         <v>128</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="10">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
         <v>125</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="10">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
         <v>167</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -1046,34 +1051,33 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="10">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
         <v>11</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -1102,34 +1106,33 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="10">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
         <v>121</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="9" t="s">
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1158,55 +1161,86 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="10">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
         <v>424</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="10">
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7">
         <v>567</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="11"/>
+      <c r="F19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
last of the sliding window neetcodes
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BE0D8-71EE-49A5-BAC4-6E316F82A73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102D4BBC-89C5-4F1D-94F1-C106D58495BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -258,6 +258,21 @@
   </si>
   <si>
     <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>Another tough one.</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t>Arrays, Sliding Window, Queue</t>
+  </si>
+  <si>
+    <t>07/06/2025</t>
+  </si>
+  <si>
+    <t>Using a special kind of Queue called a Deque in Python. We're using a Monotonically Decreasing Queue.</t>
   </si>
 </sst>
 </file>
@@ -669,27 +684,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="83.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="83.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -718,7 +733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -770,7 +785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -796,7 +811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -822,7 +837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -851,7 +866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -877,7 +892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -906,7 +921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -935,7 +950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -964,7 +979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1022,7 +1037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -1051,7 +1066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -1106,7 +1121,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1190,7 +1205,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1219,27 +1234,62 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="7">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="F20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>72</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="7">
+        <v>239</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A couple more mediums
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F8DB28-1F92-4E94-BA48-F180BB990195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1116C35D-F08F-420A-95FB-55107AF344AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="99">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -291,6 +291,48 @@
   </si>
   <si>
     <t>Smashed it.</t>
+  </si>
+  <si>
+    <t>09/06/2025</t>
+  </si>
+  <si>
+    <t>Made a silly mistake. It's quite simple actually.</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>Generate Parenthesis</t>
+  </si>
+  <si>
+    <t>10/06/2025</t>
+  </si>
+  <si>
+    <t>Stacks, Backtracking, Recursion</t>
+  </si>
+  <si>
+    <t>Why do I struggle with recursion so much?</t>
+  </si>
+  <si>
+    <t>Daily Temperatures</t>
+  </si>
+  <si>
+    <t>11/06/2025</t>
+  </si>
+  <si>
+    <t>Arrays, Stacks</t>
+  </si>
+  <si>
+    <t>Car Fleet</t>
+  </si>
+  <si>
+    <t>12/06/2025</t>
+  </si>
+  <si>
+    <t>Killed it. Did it simpler than Neetcode even!</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
   </si>
 </sst>
 </file>
@@ -689,11 +731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,6 +1397,139 @@
         <v>84</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="4">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4">
+        <v>739</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4">
+        <v>853</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Last of the stack neetcodes
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1116C35D-F08F-420A-95FB-55107AF344AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C426D9-677A-43C9-B35C-14F5453A93A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>13/06/2025</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>14/06/2025</t>
   </si>
 </sst>
 </file>
@@ -731,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1529,6 +1538,38 @@
       <c r="F28" t="s">
         <v>7</v>
       </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="4">
+        <v>704</v>
+      </c>
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Another binary search fun challenge
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660F9965-4ADB-4348-8F61-ACB5EA27AE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95FC11F-3398-45CF-B775-7ED2B3DDA241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="107">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>Killed it.</t>
+  </si>
+  <si>
+    <t>Fun one.</t>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
   </si>
 </sst>
 </file>
@@ -749,11 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1615,6 +1621,35 @@
         <v>104</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="4">
+        <v>875</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More binary search leetcodes.
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95FC11F-3398-45CF-B775-7ED2B3DDA241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4686444-8445-4D8A-B66D-926A1635A717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="113">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -357,6 +357,24 @@
   </si>
   <si>
     <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Arrays, Binary Search</t>
+  </si>
+  <si>
+    <t>16/06/2025</t>
+  </si>
+  <si>
+    <t>Struggled to handle all use cases.</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Easy once you have the simple technique.</t>
   </si>
 </sst>
 </file>
@@ -755,27 +773,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="83.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="83.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -830,7 +848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -856,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -882,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -908,7 +926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -937,7 +955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -963,7 +981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -992,7 +1010,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1068,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1079,7 +1097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1137,7 +1155,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1163,7 +1181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1218,7 +1236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1276,7 +1294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1323,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1334,7 +1352,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1363,7 +1381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1410,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1421,7 +1439,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1450,7 +1468,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1479,7 +1497,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1534,7 +1552,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1581,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1574,7 +1592,7 @@
         <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -1592,7 +1610,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1603,7 +1621,7 @@
         <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
@@ -1621,7 +1639,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1632,7 +1650,7 @@
         <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
@@ -1648,6 +1666,64 @@
       </c>
       <c r="I31" s="5" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4">
+        <v>153</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Smashing binary search now!
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4686444-8445-4D8A-B66D-926A1635A717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C510645A-78C9-4544-B48C-8273BA616A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="116">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>Easy once you have the simple technique.</t>
+  </si>
+  <si>
+    <t>Time Based Key-Value Store</t>
+  </si>
+  <si>
+    <t>Hashmaps, Binary Search</t>
+  </si>
+  <si>
+    <t>17/06/2025</t>
   </si>
 </sst>
 </file>
@@ -773,11 +782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,6 +1735,35 @@
         <v>112</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4">
+        <v>981</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
linked lists...must push through the pain!
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C510645A-78C9-4544-B48C-8273BA616A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA363E2-5629-42E1-AD5A-82D8C57BB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="127">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -384,6 +384,39 @@
   </si>
   <si>
     <t>17/06/2025</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>DEFERRED</t>
+  </si>
+  <si>
+    <t>Sticking with Easy and Medium for now.</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Linked lists…I'm scared!</t>
+  </si>
+  <si>
+    <t>Linked Lists, Two Pointers, Recursion</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Linked Lists</t>
+  </si>
+  <si>
+    <t>Neetcod 150</t>
+  </si>
+  <si>
+    <t>18/06/2025</t>
+  </si>
+  <si>
+    <t>Making a bit more sense.</t>
   </si>
 </sst>
 </file>
@@ -782,11 +815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,6 +1797,90 @@
         <v>84</v>
       </c>
     </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="4">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4">
+        <v>206</v>
+      </c>
+      <c r="C36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" t="s">
+        <v>115</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="4">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
another linked list solution
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA363E2-5629-42E1-AD5A-82D8C57BB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25585E2D-7203-47C9-A183-BEC25381D92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-23148" yWindow="456" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -410,13 +410,19 @@
     <t>Linked Lists</t>
   </si>
   <si>
-    <t>Neetcod 150</t>
-  </si>
-  <si>
     <t>18/06/2025</t>
   </si>
   <si>
     <t>Making a bit more sense.</t>
+  </si>
+  <si>
+    <t>Reorder List</t>
+  </si>
+  <si>
+    <t>Using an array seemed to help a lot. Trick was to remember how saving linked list in place works.</t>
+  </si>
+  <si>
+    <t>Remove Nth Node from End of List</t>
   </si>
 </sst>
 </file>
@@ -815,11 +821,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,16 +1875,65 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
         <v>56</v>
       </c>
       <c r="H37" t="s">
+        <v>124</v>
+      </c>
+      <c r="I37" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="I37" s="5" t="s">
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="4">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
         <v>126</v>
+      </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H38" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more linked lists challenges solved.
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25585E2D-7203-47C9-A183-BEC25381D92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F6E54D-D795-4FC1-AF5D-5272FEA3B9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="456" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="137">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -423,6 +423,30 @@
   </si>
   <si>
     <t>Remove Nth Node from End of List</t>
+  </si>
+  <si>
+    <t>19/06/2025</t>
+  </si>
+  <si>
+    <t>Linked Lists, Two Pointers</t>
+  </si>
+  <si>
+    <t>After looking at the solution it's not that bad. Clearly my mind still needs to get used to this data structure!</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>20/06/2025</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>I actually enjoyed this one!</t>
   </si>
 </sst>
 </file>
@@ -821,11 +845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1940,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1927,13 +1951,77 @@
         <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
         <v>21</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4">
+        <v>138</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last of linked lists challenges. Started Binary Tree challenges.
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F6E54D-D795-4FC1-AF5D-5272FEA3B9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D56EE-27B1-46F6-84EA-08CB292AD90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="155">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -447,6 +447,60 @@
   </si>
   <si>
     <t>I actually enjoyed this one!</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Hashmap for O(n) memory. Floyd's Toroise and Hare O(1) memory.</t>
+  </si>
+  <si>
+    <t>Find the Duplicate Number</t>
+  </si>
+  <si>
+    <t>Floyd's Toroise and Hare O(1) memory. Considered Hard.</t>
+  </si>
+  <si>
+    <t>23/06/2025</t>
+  </si>
+  <si>
+    <t>22/06/2025</t>
+  </si>
+  <si>
+    <t>Doubly Linked List</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>24/06/2025</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Diameter of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree, DFS, Recursion</t>
+  </si>
+  <si>
+    <t>Binary Tree, DFS, BFS</t>
   </si>
 </sst>
 </file>
@@ -476,12 +530,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -496,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -509,6 +569,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -845,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD42"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,6 +2098,765 @@
         <v>136</v>
       </c>
     </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4">
+        <v>141</v>
+      </c>
+      <c r="C42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s">
+        <v>142</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="4">
+        <v>287</v>
+      </c>
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H43" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="10">
+        <v>146</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="11"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="4">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="4">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="4">
+        <v>226</v>
+      </c>
+      <c r="C47" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="4">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="4">
+        <v>543</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="4">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="4">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="4">
+        <v>572</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="7"/>
+      <c r="I152" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added graph visualiser. More graph algorithms.
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB67EFC-0172-4B77-9F5B-CEA95F00934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21DBEAB-DA9D-469D-A749-8C78EE27205C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="261">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -789,6 +789,36 @@
   </si>
   <si>
     <t>25/07/2025</t>
+  </si>
+  <si>
+    <t>Graphs, BFS</t>
+  </si>
+  <si>
+    <t>Similar to Rotting Oranges above. Reverse thinking.</t>
+  </si>
+  <si>
+    <t>26/07/2025</t>
+  </si>
+  <si>
+    <t>Cycle detection.</t>
+  </si>
+  <si>
+    <t>Graphs, DFS, BFS</t>
+  </si>
+  <si>
+    <t>Course Schedule II</t>
+  </si>
+  <si>
+    <t>Topological Sort</t>
+  </si>
+  <si>
+    <t>Redundant Connection</t>
+  </si>
+  <si>
+    <t>Union Find</t>
+  </si>
+  <si>
+    <t>Number of Connected Components in Undirected Graph</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1234,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,13 +3636,16 @@
         <v>232</v>
       </c>
       <c r="D86" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="E86" t="s">
         <v>21</v>
       </c>
       <c r="F86" t="s">
         <v>7</v>
+      </c>
+      <c r="G86" t="s">
+        <v>52</v>
       </c>
       <c r="H86" t="s">
         <v>250</v>
@@ -3629,13 +3662,22 @@
         <v>233</v>
       </c>
       <c r="D87" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="E87" t="s">
         <v>21</v>
       </c>
       <c r="F87" t="s">
         <v>7</v>
+      </c>
+      <c r="G87" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" t="s">
+        <v>250</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,19 +3691,40 @@
         <v>234</v>
       </c>
       <c r="D88" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
         <v>21</v>
       </c>
       <c r="F88" t="s">
         <v>7</v>
+      </c>
+      <c r="G88" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s">
+        <v>253</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>5</v>
       </c>
+      <c r="B89" s="4">
+        <v>210</v>
+      </c>
+      <c r="C89" t="s">
+        <v>256</v>
+      </c>
+      <c r="D89" t="s">
+        <v>257</v>
+      </c>
+      <c r="E89" t="s">
+        <v>21</v>
+      </c>
       <c r="F89" t="s">
         <v>7</v>
       </c>
@@ -3670,6 +3733,15 @@
       <c r="A90" t="s">
         <v>5</v>
       </c>
+      <c r="B90" s="4">
+        <v>684</v>
+      </c>
+      <c r="C90" t="s">
+        <v>258</v>
+      </c>
+      <c r="D90" t="s">
+        <v>259</v>
+      </c>
       <c r="F90" t="s">
         <v>7</v>
       </c>
@@ -3677,6 +3749,15 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
+      </c>
+      <c r="B91" s="4">
+        <v>323</v>
+      </c>
+      <c r="C91" t="s">
+        <v>260</v>
+      </c>
+      <c r="D91" t="s">
+        <v>259</v>
       </c>
       <c r="F91" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Completed DP challengs. Onto Greedy algorithms.
</commit_message>
<xml_diff>
--- a/docs/Programming Puzzles.xlsx
+++ b/docs/Programming Puzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A596251-E784-4E31-8006-35B83983C08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACC4D9D-1067-42B7-AF08-20E902BD9D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="328">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -1009,6 +1009,18 @@
   </si>
   <si>
     <t>DFS with cache.</t>
+  </si>
+  <si>
+    <t>29/08/2025</t>
+  </si>
+  <si>
+    <t>Still a bit iffy on the solution given by neetcode. Doesn't make complete sense to me.</t>
+  </si>
+  <si>
+    <t>01/09/2025</t>
+  </si>
+  <si>
+    <t>Jump Game II</t>
   </si>
 </sst>
 </file>
@@ -1435,8 +1447,8 @@
   <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4706,6 +4718,15 @@
       <c r="F117" t="s">
         <v>7</v>
       </c>
+      <c r="G117" t="s">
+        <v>51</v>
+      </c>
+      <c r="H117" t="s">
+        <v>324</v>
+      </c>
+      <c r="I117" s="5" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -4836,7 +4857,7 @@
         <v>271</v>
       </c>
       <c r="E123" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F123" t="s">
         <v>7</v>
@@ -4861,10 +4882,28 @@
       <c r="F124" t="s">
         <v>7</v>
       </c>
+      <c r="G124" t="s">
+        <v>12</v>
+      </c>
+      <c r="H124" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>5</v>
+      </c>
+      <c r="B125" s="4">
+        <v>45</v>
+      </c>
+      <c r="C125" t="s">
+        <v>327</v>
+      </c>
+      <c r="D125" t="s">
+        <v>318</v>
+      </c>
+      <c r="E125" t="s">
+        <v>21</v>
       </c>
       <c r="F125" t="s">
         <v>7</v>

</xml_diff>